<commit_message>
Same as last one
</commit_message>
<xml_diff>
--- a/Docs/Prashant Mewada.xlsx
+++ b/Docs/Prashant Mewada.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XLNC\Documents\UiPath\LinkedInBot\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prashant\Documents\UiPath\LinkedInBot\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C987E94-9500-42BD-976C-D82F8402631A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="3540" windowWidth="21600" windowHeight="11295"/>
+    <workbookView xWindow="4995" yWindow="2865" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -173,12 +174,126 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/natasha-castelino-92590b7b?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAABEK620B9eP5H9iv543swL-IiLJKb-ALHMo</t>
+  </si>
+  <si>
+    <t>Lalit ..</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/lalit-4bba7924a?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAD29Do8B6n63DBAgEUbzASH-DNU18DFXrgE</t>
+  </si>
+  <si>
+    <t>Kavya Shree</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/kavyashreeav?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAAt7G7gBZBipGj3co0ddZiNKK__1xhLBVTQ</t>
+  </si>
+  <si>
+    <t>Shwetha S L</t>
+  </si>
+  <si>
+    <t>Pending - Already Sent</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/shwetha-s-l-7904a924?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAAUOWxwB8e7Wsf6VKyY9g0OR3UwFmfLzGHA</t>
+  </si>
+  <si>
+    <t>Harshith K</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/harshith-k-455a3224b?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAD3pKwEBmHbKU2rk6XEXGbjoPGIUjyrjH8E</t>
+  </si>
+  <si>
+    <t>Hemant S</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/hemant-s-0a1a481b7?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAADKFonkBhhq0LQIoBZx7pU8v-JOFtIrAkGk</t>
+  </si>
+  <si>
+    <t>R Aarthi She/Her</t>
+  </si>
+  <si>
+    <t>Follow - Sent</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/aarthirecruitergoogle?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAABmDMYcBHai2bR4gJ9Hy7ATnN6Mv9Jrb2mA</t>
+  </si>
+  <si>
+    <t>Ankita Goel</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ankita-goel-007ab5147?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACOUhMcB24kw_osHDEw3La9F4hBGBPNpUWI</t>
+  </si>
+  <si>
+    <t>Srinath M</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/srinath-m-546651244?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAADybpsYBki2f6h7c-j4Dy7p2SoaKeUEjNWs</t>
+  </si>
+  <si>
+    <t>Vidya hj</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/vidyahj?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAABsAHJkB7r-ikZXuMH8q9Opw2TYU_pDzVdE</t>
+  </si>
+  <si>
+    <t>Anuraag Mandanna</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/anuraag-mandanna-a06b75158?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACXnYmYBc_wNWufnIVXRQLIb-_UwY9OuUCI</t>
+  </si>
+  <si>
+    <t>Ramya D</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ramya-d-b7310b106?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAABq2fMcBApC11S5AGrSeSGKVEsHnOWMATAY</t>
+  </si>
+  <si>
+    <t>Apeksha .</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/apeksha3?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAAnEoRABgpnQUOiRjkIujbUbbLCDgTNMkLw</t>
+  </si>
+  <si>
+    <t>Samreen Jabbar</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/samreen-jabbar-220239172?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACj4KPgB1-GRuUKp7Y1JW6EGeCZpfmZcxLU</t>
+  </si>
+  <si>
+    <t>Astha Handa</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/asthahanda?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACYJDAkB6F5meb0X1a8RpFMJ736SaBMosIE</t>
+  </si>
+  <si>
+    <t>Preethika gk</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/preethika-gk-b60144140?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACIxMXgBCHQlrQ2Kd6vWjCNNv_NV0HjrNr0</t>
+  </si>
+  <si>
+    <t>Sananda Basu</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sananda-basu-666a3358?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAAxBQu4B1pbluJLT08oDB_nv5r7FIefoIlg</t>
+  </si>
+  <si>
+    <t>Luzanna Virgina Barretto</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/luzanna-virgina-barretto-b170401a2?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAC9Y6kMBfuv5q1qNF5jMAsBpaz55R6SS8XU</t>
+  </si>
+  <si>
+    <t>Athiba Syed</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/athiba-syed-432923176?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACnIhKYBbKNHfAdCeQfQs1p6FsmA0198ZYs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -490,17 +605,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -560,7 +675,7 @@
         <v>44830.43886574074</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -573,9 +688,14 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44831.957442129627</v>
+      </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -588,8 +708,69 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44831.959918981483</v>
+      </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -599,8 +780,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
@@ -839,17 +1020,377 @@
         <v>44830.438807870371</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="1">
+        <v>44831.956238425926</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="1">
+        <v>44831.956284722219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="1">
+        <v>44831.956284722219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="1">
+        <v>44831.95653935185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="1">
+        <v>44831.956585648149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="1">
+        <v>44831.95684027778</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="1">
+        <v>44831.957083333335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="1">
+        <v>44831.957326388889</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="1">
+        <v>44831.957372685189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="1">
+        <v>44831.958101851851</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="1">
+        <v>44831.958333333336</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="1">
+        <v>44831.958599537036</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="1">
+        <v>44831.95884259259</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="1">
+        <v>44831.959097222221</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="1">
+        <v>44831.959340277775</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="1">
+        <v>44831.95957175926</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="1">
+        <v>44831.959618055553</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29" s="1">
+        <v>44831.959872685184</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Completed with withddraw and changes in extraction Short profile URL
</commit_message>
<xml_diff>
--- a/Docs/Prashant Mewada.xlsx
+++ b/Docs/Prashant Mewada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prashant\Documents\UiPath\LinkedInBot\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C987E94-9500-42BD-976C-D82F8402631A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDBD838-739E-4CFE-813B-CAC03A4D3226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4995" yWindow="2865" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4035" yWindow="3840" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="201">
   <si>
     <t>Name</t>
   </si>
@@ -104,190 +104,532 @@
     <t>DataTimestamp</t>
   </si>
   <si>
-    <t>Widthdrawn</t>
-  </si>
-  <si>
     <t>Nikhita Singh</t>
   </si>
   <si>
     <t>Message - Sent</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/nikhita-singh-a8423878?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAABBohwQBVxAaxnlHGcEhGYPLbUk2K4cfspM</t>
-  </si>
-  <si>
     <t>preethi kumar</t>
   </si>
   <si>
     <t>Message - Already Sent</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/preethi-kumar-533603145?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACMmrzcBuZT5gSFrQPxrZBxQK3goTwkZbDc</t>
-  </si>
-  <si>
     <t>Aishwarya BP</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/aishwarya-bp-37a059103?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAABorg84BMXvgvbAyq0JxoxyIAgk8RahvhDQ</t>
-  </si>
-  <si>
     <t>Shruthi Abbar</t>
   </si>
   <si>
     <t>Connect - Sent</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/shruthi-abbar-47685a177?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACnzaxoBySAvXwpC8YnbJwBuTWv96NXm6To</t>
-  </si>
-  <si>
     <t>RIVIN MATHEW</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/rivin-mathew-0a64b0135?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACD_u34B2Nqz595efGkVi1Nj_9ZsZo8c0TI</t>
-  </si>
-  <si>
     <t>Aarthi Raju</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/aarthi-raju-792a0b197?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAC4-9p4BTu6bJ_ft8aDkNyJyZvqS2H55-M4</t>
-  </si>
-  <si>
     <t>Smitha H</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/smitha-h-3672a2155?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACU9YX8BPJ8Jtjzq1onul_LeeohCQskIWTU</t>
-  </si>
-  <si>
     <t>Sonal Ranjit</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/sonal-ranjit-a77ba8164?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACdU6fsBWhp9QE47Xy_kT6iQQwHvNpr27b4</t>
-  </si>
-  <si>
     <t>Parul Narayan</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/parul-narayan-b551391a4?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAC-3wjEB_vXizWzTrx2OKoZwG2m9aZoFMNw</t>
-  </si>
-  <si>
     <t>Natasha Castelino</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/natasha-castelino-92590b7b?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAABEK620B9eP5H9iv543swL-IiLJKb-ALHMo</t>
-  </si>
-  <si>
     <t>Lalit ..</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/lalit-4bba7924a?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAD29Do8B6n63DBAgEUbzASH-DNU18DFXrgE</t>
-  </si>
-  <si>
     <t>Kavya Shree</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/kavyashreeav?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAAt7G7gBZBipGj3co0ddZiNKK__1xhLBVTQ</t>
-  </si>
-  <si>
     <t>Shwetha S L</t>
   </si>
   <si>
     <t>Pending - Already Sent</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/shwetha-s-l-7904a924?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAAUOWxwB8e7Wsf6VKyY9g0OR3UwFmfLzGHA</t>
-  </si>
-  <si>
     <t>Harshith K</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/harshith-k-455a3224b?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAD3pKwEBmHbKU2rk6XEXGbjoPGIUjyrjH8E</t>
-  </si>
-  <si>
     <t>Hemant S</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/hemant-s-0a1a481b7?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAADKFonkBhhq0LQIoBZx7pU8v-JOFtIrAkGk</t>
-  </si>
-  <si>
     <t>R Aarthi She/Her</t>
   </si>
   <si>
     <t>Follow - Sent</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/aarthirecruitergoogle?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAABmDMYcBHai2bR4gJ9Hy7ATnN6Mv9Jrb2mA</t>
-  </si>
-  <si>
     <t>Ankita Goel</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/ankita-goel-007ab5147?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACOUhMcB24kw_osHDEw3La9F4hBGBPNpUWI</t>
-  </si>
-  <si>
     <t>Srinath M</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/srinath-m-546651244?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAADybpsYBki2f6h7c-j4Dy7p2SoaKeUEjNWs</t>
-  </si>
-  <si>
     <t>Vidya hj</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/vidyahj?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAABsAHJkB7r-ikZXuMH8q9Opw2TYU_pDzVdE</t>
-  </si>
-  <si>
     <t>Anuraag Mandanna</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/anuraag-mandanna-a06b75158?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACXnYmYBc_wNWufnIVXRQLIb-_UwY9OuUCI</t>
-  </si>
-  <si>
     <t>Ramya D</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/ramya-d-b7310b106?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAABq2fMcBApC11S5AGrSeSGKVEsHnOWMATAY</t>
-  </si>
-  <si>
     <t>Apeksha .</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/apeksha3?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAAnEoRABgpnQUOiRjkIujbUbbLCDgTNMkLw</t>
-  </si>
-  <si>
     <t>Samreen Jabbar</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/samreen-jabbar-220239172?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACj4KPgB1-GRuUKp7Y1JW6EGeCZpfmZcxLU</t>
-  </si>
-  <si>
     <t>Astha Handa</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/asthahanda?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACYJDAkB6F5meb0X1a8RpFMJ736SaBMosIE</t>
-  </si>
-  <si>
     <t>Preethika gk</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/preethika-gk-b60144140?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACIxMXgBCHQlrQ2Kd6vWjCNNv_NV0HjrNr0</t>
-  </si>
-  <si>
     <t>Sananda Basu</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/sananda-basu-666a3358?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAAxBQu4B1pbluJLT08oDB_nv5r7FIefoIlg</t>
-  </si>
-  <si>
     <t>Luzanna Virgina Barretto</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/luzanna-virgina-barretto-b170401a2?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAAC9Y6kMBfuv5q1qNF5jMAsBpaz55R6SS8XU</t>
-  </si>
-  <si>
     <t>Athiba Syed</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/athiba-syed-432923176?miniProfileUrn=urn%3Ali%3Afs_miniProfile%3AACoAACnIhKYBbKNHfAdCeQfQs1p6FsmA0198ZYs</t>
+    <t>Withdrawn</t>
+  </si>
+  <si>
+    <t>WithdrawTimeStamp</t>
+  </si>
+  <si>
+    <t>Srinivasulu Neeruganti</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/srinivasulu-neeruganti-632386b/</t>
+  </si>
+  <si>
+    <t>Withdraw</t>
+  </si>
+  <si>
+    <t>Philomena Lincy</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/philomena-lincy-2b7a4610/</t>
+  </si>
+  <si>
+    <t>Antarikhya Deka</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/antarikhya-deka-ab0ba169/</t>
+  </si>
+  <si>
+    <t>Sangram Guha</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sangram-guha-6ba27634/</t>
+  </si>
+  <si>
+    <t>Khushboo Sinha</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/khushboo-sinha-74252338/</t>
+  </si>
+  <si>
+    <t>Snigdha Mukherjee</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/snigdha-mukherjee-7998b4154/</t>
+  </si>
+  <si>
+    <t>Sandhya Tiwari</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sandhya-tiwari-27838a56/</t>
+  </si>
+  <si>
+    <t>Soma Dutta</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/soma-dutta-b6b343194/</t>
+  </si>
+  <si>
+    <t>Revathi D.</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/revathi-d-64807a6/</t>
+  </si>
+  <si>
+    <t>Manushi Sharma</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/manushi-sharma-56923a120/</t>
+  </si>
+  <si>
+    <t>Vishnu Arumugam</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/vishnu-arumugam-a470216a/</t>
+  </si>
+  <si>
+    <t>Srushti Shah</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/srushtishah-leadership-hiring/</t>
+  </si>
+  <si>
+    <t>Apoorv Katiyar</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/apoorv-katiyar-82776118b/</t>
+  </si>
+  <si>
+    <t>Gangadhar Salimath</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/gangadharsalimath/</t>
+  </si>
+  <si>
+    <t>Rakhi Chadaga</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/rakhi-chadaga-a9539120/</t>
+  </si>
+  <si>
+    <t>Reuben R.</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/reubenrraj/</t>
+  </si>
+  <si>
+    <t>Mahjabin Fatma</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/mahjabinfatma/</t>
+  </si>
+  <si>
+    <t>Rubi Kumar</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/rubi-kumar-17a20242/</t>
+  </si>
+  <si>
+    <t>Steve Bulls ~ Skilled RPA and Excel VBA Programmer</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/steve-bulls/</t>
+  </si>
+  <si>
+    <t>Priya Rajput</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/priya-rajput-2729ba224/</t>
+  </si>
+  <si>
+    <t>Anisha Sahu</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/anishasahu96/</t>
+  </si>
+  <si>
+    <t>Payel Biswas</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/payel-biswas-17ab53119/</t>
+  </si>
+  <si>
+    <t>Harshitha Raju</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/harshitha-raju/</t>
+  </si>
+  <si>
+    <t>Kajal Dash</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/kajal-dash-7574a2103/</t>
+  </si>
+  <si>
+    <t>Chanchala Ugra</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/chanchala-ugra-a44029145/</t>
+  </si>
+  <si>
+    <t>Akashdeep Bhowal</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/akashdeep-bhowal-b43b51104/</t>
+  </si>
+  <si>
+    <t>AMULYA V R.</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/amulyavrao/</t>
+  </si>
+  <si>
+    <t>Niveditha Rao</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/niveditha-rao-b5b9881a3/</t>
+  </si>
+  <si>
+    <t>Trishita K.</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/trishita-k-9666891ab/</t>
+  </si>
+  <si>
+    <t>Prashanth Bharadwaj</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/prashanth-bharadwaj-7a67b950/</t>
+  </si>
+  <si>
+    <t>Cheruku Sabarish</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/cherukusabarish/</t>
+  </si>
+  <si>
+    <t>Samatha Krishna</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/samatha-krishna-91a3b3175/</t>
+  </si>
+  <si>
+    <t>Deepthi Nandina</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/deepthi-nandina-10226a164/</t>
+  </si>
+  <si>
+    <t>Nikitha Lingaraju</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/nikitha-lingaraju-966903172/</t>
+  </si>
+  <si>
+    <t>Khushbu Roy</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/khushbu-roy-2209/</t>
+  </si>
+  <si>
+    <t>Puja rajak</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/puja-rajak-98b14914a/</t>
+  </si>
+  <si>
+    <t>Kundan Yadav</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/kundan-yadav-6a490984/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/nikhita-singh-a8423878</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/preethi-kumar-533603145</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/aishwarya-bp-37a059103</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/shruthi-abbar-47685a177</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/rivin-mathew-0a64b0135</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/aarthi-raju-792a0b197</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/smitha-h-3672a2155</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sonal-ranjit-a77ba8164</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/parul-narayan-b551391a4</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/natasha-castelino-92590b7b</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/lalit-4bba7924a</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/kavyashreeav</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/shwetha-s-l-7904a924</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/harshith-k-455a3224b</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/hemant-s-0a1a481b7</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/aarthirecruitergoogle</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ankita-goel-007ab5147</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/srinath-m-546651244</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/vidyahj</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/anuraag-mandanna-a06b75158</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ramya-d-b7310b106</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/apeksha3</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/samreen-jabbar-220239172</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/asthahanda</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/preethika-gk-b60144140</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sananda-basu-666a3358</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/luzanna-virgina-barretto-b170401a2</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/athiba-syed-432923176</t>
+  </si>
+  <si>
+    <t>Aiyappa B R</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/aiyappa-b-r-195a9b17</t>
+  </si>
+  <si>
+    <t>Monica Lokare</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/monica-lokare-9549a3146</t>
+  </si>
+  <si>
+    <t>Swetha Shivakumar</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/swetha-shivakumar-3284b213</t>
+  </si>
+  <si>
+    <t>Asha Rani D M</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/asha-rani-d-m-a070521b6</t>
+  </si>
+  <si>
+    <t>Sweta Yadav</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/iamswetayadav</t>
+  </si>
+  <si>
+    <t>Chitranshi Saxena</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/chitranshi-saxena-274b7015a</t>
+  </si>
+  <si>
+    <t>Keerthana Balasubramaniam</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/keerthana-balasubramaniam</t>
+  </si>
+  <si>
+    <t>Abhirami Sivan</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/abhirami-sivan-07822615b</t>
+  </si>
+  <si>
+    <t>Udaya Bhaskar</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/udayabhaskar</t>
+  </si>
+  <si>
+    <t>Debaroti Roy</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/debaroti-roy-b0a68479</t>
+  </si>
+  <si>
+    <t>Lekha Sree D</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/lekha-sree-d-77761724a</t>
+  </si>
+  <si>
+    <t>Abirami Manoharan</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/abirami-manoharan-a919bb196</t>
+  </si>
+  <si>
+    <t>Bhavana Arya</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/bhavana-arya-72515a170</t>
+  </si>
+  <si>
+    <t>Gayathri Anbumathi</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/gayathri-anbumathi-3a399423b</t>
+  </si>
+  <si>
+    <t>Akash T</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/akash-t-392897248</t>
+  </si>
+  <si>
+    <t>Ramya Chendaluru</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ramya-chendaluru-a6383a153</t>
+  </si>
+  <si>
+    <t>Abishai c</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/abishai-c-721816246</t>
+  </si>
+  <si>
+    <t>Bhakti Choudhari</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/bhakti-choudhari-0b75b4247</t>
+  </si>
+  <si>
+    <t>Mamta Nanda</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/mamta-nanda-0a9b7a23a</t>
   </si>
 </sst>
 </file>
@@ -609,7 +951,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +1037,7 @@
         <v>44831.957442129627</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -715,7 +1057,7 @@
         <v>44831.959918981483</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -728,6 +1070,15 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44833.883576388886</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -738,6 +1089,15 @@
       </c>
       <c r="C7" t="s">
         <v>12</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44833.88616898148</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -781,11 +1141,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -795,9 +1153,10 @@
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -817,12 +1176,15 @@
         <v>24</v>
       </c>
       <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -831,18 +1193,18 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>135</v>
       </c>
       <c r="F2" s="1">
         <v>44830.40488425926</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -851,18 +1213,18 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="F3" s="1">
         <v>44830.404988425929</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -871,18 +1233,18 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>137</v>
       </c>
       <c r="F4" s="1">
         <v>44830.40525462963</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -891,18 +1253,18 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>138</v>
       </c>
       <c r="F5" s="1">
         <v>44830.405300925922</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -911,18 +1273,18 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>139</v>
       </c>
       <c r="F6" s="1">
         <v>44830.405347222222</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -931,18 +1293,18 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="F7" s="1">
         <v>44830.437939814816</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -951,18 +1313,18 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>141</v>
       </c>
       <c r="F8" s="1">
         <v>44830.438217592593</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -971,18 +1333,18 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="F9" s="1">
         <v>44830.43849537037</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -991,18 +1353,18 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>143</v>
       </c>
       <c r="F10" s="1">
         <v>44830.438761574071</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1011,18 +1373,18 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>144</v>
       </c>
       <c r="F11" s="1">
         <v>44830.438807870371</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -1031,18 +1393,18 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="F12" s="1">
         <v>44831.956238425926</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
@@ -1051,18 +1413,18 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="F13" s="1">
         <v>44831.956284722219</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -1071,18 +1433,24 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>147</v>
       </c>
       <c r="F14" s="1">
         <v>44831.956284722219</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="1">
+        <v>44833.857303240744</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -1091,18 +1459,18 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="F15" s="1">
         <v>44831.95653935185</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -1111,18 +1479,18 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>149</v>
       </c>
       <c r="F16" s="1">
         <v>44831.956585648149</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
@@ -1131,18 +1499,18 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>150</v>
       </c>
       <c r="F17" s="1">
         <v>44831.95684027778</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -1151,18 +1519,18 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>151</v>
       </c>
       <c r="F18" s="1">
         <v>44831.957083333335</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
@@ -1171,18 +1539,18 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>152</v>
       </c>
       <c r="F19" s="1">
         <v>44831.957326388889</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
@@ -1191,18 +1559,18 @@
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>153</v>
       </c>
       <c r="F20" s="1">
         <v>44831.957372685189</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
@@ -1211,18 +1579,18 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
+        <v>154</v>
       </c>
       <c r="F21" s="1">
         <v>44831.958101851851</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
         <v>17</v>
@@ -1231,18 +1599,18 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>155</v>
       </c>
       <c r="F22" s="1">
         <v>44831.958333333336</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
@@ -1251,18 +1619,18 @@
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>156</v>
       </c>
       <c r="F23" s="1">
         <v>44831.958599537036</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
@@ -1271,18 +1639,18 @@
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>157</v>
       </c>
       <c r="F24" s="1">
         <v>44831.95884259259</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
         <v>17</v>
@@ -1291,18 +1659,18 @@
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>158</v>
       </c>
       <c r="F25" s="1">
         <v>44831.959097222221</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
         <v>17</v>
@@ -1311,18 +1679,18 @@
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
+        <v>159</v>
       </c>
       <c r="F26" s="1">
         <v>44831.959340277775</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
         <v>17</v>
@@ -1331,18 +1699,18 @@
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>82</v>
+        <v>160</v>
       </c>
       <c r="F27" s="1">
         <v>44831.95957175926</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
         <v>17</v>
@@ -1351,18 +1719,18 @@
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="F28" s="1">
         <v>44831.959618055553</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
         <v>17</v>
@@ -1371,13 +1739,911 @@
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E29" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="F29" s="1">
         <v>44831.959872685184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H30" s="1">
+        <v>44833.855821759258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" t="s">
+        <v>62</v>
+      </c>
+      <c r="H31" s="1">
+        <v>44833.856261574074</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32" t="s">
+        <v>62</v>
+      </c>
+      <c r="H32" s="1">
+        <v>44833.856956018521</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" t="s">
+        <v>62</v>
+      </c>
+      <c r="H33" s="1">
+        <v>44833.85701388889</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" t="s">
+        <v>70</v>
+      </c>
+      <c r="G34" t="s">
+        <v>62</v>
+      </c>
+      <c r="H34" s="1">
+        <v>44833.857071759259</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" t="s">
+        <v>72</v>
+      </c>
+      <c r="G35" t="s">
+        <v>62</v>
+      </c>
+      <c r="H35" s="1">
+        <v>44833.857129629629</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" t="s">
+        <v>74</v>
+      </c>
+      <c r="G36" t="s">
+        <v>62</v>
+      </c>
+      <c r="H36" s="1">
+        <v>44833.857187499998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="E37" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" t="s">
+        <v>62</v>
+      </c>
+      <c r="H37" s="1">
+        <v>44833.857245370367</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" t="s">
+        <v>62</v>
+      </c>
+      <c r="H38" s="1">
+        <v>44833.857581018521</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" t="s">
+        <v>80</v>
+      </c>
+      <c r="G39" t="s">
+        <v>62</v>
+      </c>
+      <c r="H39" s="1">
+        <v>44833.857638888891</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>81</v>
+      </c>
+      <c r="E40" t="s">
+        <v>82</v>
+      </c>
+      <c r="G40" t="s">
+        <v>62</v>
+      </c>
+      <c r="H40" s="1">
+        <v>44833.85769675926</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41" t="s">
+        <v>84</v>
+      </c>
+      <c r="G41" t="s">
+        <v>62</v>
+      </c>
+      <c r="H41" s="1">
+        <v>44833.857754629629</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="E42" t="s">
+        <v>86</v>
+      </c>
+      <c r="G42" t="s">
+        <v>62</v>
+      </c>
+      <c r="H42" s="1">
+        <v>44833.857812499999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G43" t="s">
+        <v>62</v>
+      </c>
+      <c r="H43" s="1">
+        <v>44833.857870370368</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" t="s">
+        <v>90</v>
+      </c>
+      <c r="G44" t="s">
+        <v>62</v>
+      </c>
+      <c r="H44" s="1">
+        <v>44833.857928240737</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="E45" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" t="s">
+        <v>62</v>
+      </c>
+      <c r="H45" s="1">
+        <v>44833.857986111114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>93</v>
+      </c>
+      <c r="E46" t="s">
+        <v>94</v>
+      </c>
+      <c r="G46" t="s">
+        <v>62</v>
+      </c>
+      <c r="H46" s="1">
+        <v>44833.858043981483</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E47" t="s">
+        <v>96</v>
+      </c>
+      <c r="G47" t="s">
+        <v>62</v>
+      </c>
+      <c r="H47" s="1">
+        <v>44833.858101851853</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+      <c r="E48" t="s">
+        <v>98</v>
+      </c>
+      <c r="G48" t="s">
+        <v>62</v>
+      </c>
+      <c r="H48" s="1">
+        <v>44833.858159722222</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>99</v>
+      </c>
+      <c r="E49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G49" t="s">
+        <v>62</v>
+      </c>
+      <c r="H49" s="1">
+        <v>44833.858217592591</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" t="s">
+        <v>102</v>
+      </c>
+      <c r="G50" t="s">
+        <v>62</v>
+      </c>
+      <c r="H50" s="1">
+        <v>44833.858275462961</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" t="s">
+        <v>104</v>
+      </c>
+      <c r="G51" t="s">
+        <v>62</v>
+      </c>
+      <c r="H51" s="1">
+        <v>44833.85833333333</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>105</v>
+      </c>
+      <c r="E52" t="s">
+        <v>106</v>
+      </c>
+      <c r="G52" t="s">
+        <v>62</v>
+      </c>
+      <c r="H52" s="1">
+        <v>44833.858391203707</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>107</v>
+      </c>
+      <c r="E53" t="s">
+        <v>108</v>
+      </c>
+      <c r="G53" t="s">
+        <v>62</v>
+      </c>
+      <c r="H53" s="1">
+        <v>44833.858449074076</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>109</v>
+      </c>
+      <c r="E54" t="s">
+        <v>110</v>
+      </c>
+      <c r="G54" t="s">
+        <v>62</v>
+      </c>
+      <c r="H54" s="1">
+        <v>44833.858506944445</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>111</v>
+      </c>
+      <c r="E55" t="s">
+        <v>112</v>
+      </c>
+      <c r="G55" t="s">
+        <v>62</v>
+      </c>
+      <c r="H55" s="1">
+        <v>44833.858564814815</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>113</v>
+      </c>
+      <c r="E56" t="s">
+        <v>114</v>
+      </c>
+      <c r="G56" t="s">
+        <v>62</v>
+      </c>
+      <c r="H56" s="1">
+        <v>44833.858622685184</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>115</v>
+      </c>
+      <c r="E57" t="s">
+        <v>116</v>
+      </c>
+      <c r="G57" t="s">
+        <v>62</v>
+      </c>
+      <c r="H57" s="1">
+        <v>44833.858680555553</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>117</v>
+      </c>
+      <c r="E58" t="s">
+        <v>118</v>
+      </c>
+      <c r="G58" t="s">
+        <v>62</v>
+      </c>
+      <c r="H58" s="1">
+        <v>44833.858738425923</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>119</v>
+      </c>
+      <c r="E59" t="s">
+        <v>120</v>
+      </c>
+      <c r="G59" t="s">
+        <v>62</v>
+      </c>
+      <c r="H59" s="1">
+        <v>44833.858796296299</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>121</v>
+      </c>
+      <c r="E60" t="s">
+        <v>122</v>
+      </c>
+      <c r="G60" t="s">
+        <v>62</v>
+      </c>
+      <c r="H60" s="1">
+        <v>44833.858854166669</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+      <c r="E61" t="s">
+        <v>124</v>
+      </c>
+      <c r="G61" t="s">
+        <v>62</v>
+      </c>
+      <c r="H61" s="1">
+        <v>44833.858912037038</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>125</v>
+      </c>
+      <c r="E62" t="s">
+        <v>126</v>
+      </c>
+      <c r="G62" t="s">
+        <v>62</v>
+      </c>
+      <c r="H62" s="1">
+        <v>44833.858969907407</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>127</v>
+      </c>
+      <c r="E63" t="s">
+        <v>128</v>
+      </c>
+      <c r="G63" t="s">
+        <v>62</v>
+      </c>
+      <c r="H63" s="1">
+        <v>44833.859027777777</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>129</v>
+      </c>
+      <c r="E64" t="s">
+        <v>130</v>
+      </c>
+      <c r="G64" t="s">
+        <v>62</v>
+      </c>
+      <c r="H64" s="1">
+        <v>44833.859085648146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>131</v>
+      </c>
+      <c r="E65" t="s">
+        <v>132</v>
+      </c>
+      <c r="G65" t="s">
+        <v>62</v>
+      </c>
+      <c r="H65" s="1">
+        <v>44833.859143518515</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>133</v>
+      </c>
+      <c r="E66" t="s">
+        <v>134</v>
+      </c>
+      <c r="G66" t="s">
+        <v>62</v>
+      </c>
+      <c r="H66" s="1">
+        <v>44833.859189814815</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>163</v>
+      </c>
+      <c r="B67" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" t="s">
+        <v>45</v>
+      </c>
+      <c r="E67" t="s">
+        <v>164</v>
+      </c>
+      <c r="F67" s="1">
+        <v>44833.882372685184</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>165</v>
+      </c>
+      <c r="B68" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
+        <v>26</v>
+      </c>
+      <c r="E68" t="s">
+        <v>166</v>
+      </c>
+      <c r="F68" s="1">
+        <v>44833.882638888892</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>167</v>
+      </c>
+      <c r="B69" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" t="s">
+        <v>31</v>
+      </c>
+      <c r="E69" t="s">
+        <v>168</v>
+      </c>
+      <c r="F69" s="1">
+        <v>44833.882708333331</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>169</v>
+      </c>
+      <c r="B70" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" t="s">
+        <v>31</v>
+      </c>
+      <c r="E70" t="s">
+        <v>170</v>
+      </c>
+      <c r="F70" s="1">
+        <v>44833.882777777777</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>171</v>
+      </c>
+      <c r="B71" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" t="s">
+        <v>31</v>
+      </c>
+      <c r="E71" t="s">
+        <v>172</v>
+      </c>
+      <c r="F71" s="1">
+        <v>44833.882835648146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>173</v>
+      </c>
+      <c r="B72" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" t="s">
+        <v>174</v>
+      </c>
+      <c r="F72" s="1">
+        <v>44833.883113425924</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>175</v>
+      </c>
+      <c r="B73" t="s">
+        <v>19</v>
+      </c>
+      <c r="C73" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" t="s">
+        <v>31</v>
+      </c>
+      <c r="E73" t="s">
+        <v>176</v>
+      </c>
+      <c r="F73" s="1">
+        <v>44833.88318287037</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>177</v>
+      </c>
+      <c r="B74" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" t="s">
+        <v>26</v>
+      </c>
+      <c r="E74" t="s">
+        <v>178</v>
+      </c>
+      <c r="F74" s="1">
+        <v>44833.883449074077</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>179</v>
+      </c>
+      <c r="B75" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" t="s">
+        <v>31</v>
+      </c>
+      <c r="E75" t="s">
+        <v>180</v>
+      </c>
+      <c r="F75" s="1">
+        <v>44833.883518518516</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>181</v>
+      </c>
+      <c r="B76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" t="s">
+        <v>31</v>
+      </c>
+      <c r="E76" t="s">
+        <v>182</v>
+      </c>
+      <c r="F76" s="1">
+        <v>44833.884085648147</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>183</v>
+      </c>
+      <c r="B77" t="s">
+        <v>20</v>
+      </c>
+      <c r="C77" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" t="s">
+        <v>26</v>
+      </c>
+      <c r="E77" t="s">
+        <v>184</v>
+      </c>
+      <c r="F77" s="1">
+        <v>44833.884351851855</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>185</v>
+      </c>
+      <c r="B78" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" t="s">
+        <v>31</v>
+      </c>
+      <c r="E78" t="s">
+        <v>186</v>
+      </c>
+      <c r="F78" s="1">
+        <v>44833.884421296294</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>187</v>
+      </c>
+      <c r="B79" t="s">
+        <v>20</v>
+      </c>
+      <c r="C79" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" t="s">
+        <v>31</v>
+      </c>
+      <c r="E79" t="s">
+        <v>188</v>
+      </c>
+      <c r="F79" s="1">
+        <v>44833.88449074074</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>189</v>
+      </c>
+      <c r="B80" t="s">
+        <v>20</v>
+      </c>
+      <c r="C80" t="s">
+        <v>12</v>
+      </c>
+      <c r="D80" t="s">
+        <v>31</v>
+      </c>
+      <c r="E80" t="s">
+        <v>190</v>
+      </c>
+      <c r="F80" s="1">
+        <v>44833.884560185186</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>191</v>
+      </c>
+      <c r="B81" t="s">
+        <v>20</v>
+      </c>
+      <c r="C81" t="s">
+        <v>12</v>
+      </c>
+      <c r="D81" t="s">
+        <v>26</v>
+      </c>
+      <c r="E81" t="s">
+        <v>192</v>
+      </c>
+      <c r="F81" s="1">
+        <v>44833.884814814817</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>193</v>
+      </c>
+      <c r="B82" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" t="s">
+        <v>12</v>
+      </c>
+      <c r="D82" t="s">
+        <v>31</v>
+      </c>
+      <c r="E82" t="s">
+        <v>194</v>
+      </c>
+      <c r="F82" s="1">
+        <v>44833.884884259256</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>195</v>
+      </c>
+      <c r="B83" t="s">
+        <v>20</v>
+      </c>
+      <c r="C83" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83" t="s">
+        <v>26</v>
+      </c>
+      <c r="E83" t="s">
+        <v>196</v>
+      </c>
+      <c r="F83" s="1">
+        <v>44833.885150462964</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>197</v>
+      </c>
+      <c r="B84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C84" t="s">
+        <v>12</v>
+      </c>
+      <c r="D84" t="s">
+        <v>45</v>
+      </c>
+      <c r="E84" t="s">
+        <v>198</v>
+      </c>
+      <c r="F84" s="1">
+        <v>44833.885833333334</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>199</v>
+      </c>
+      <c r="B85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C85" t="s">
+        <v>12</v>
+      </c>
+      <c r="D85" t="s">
+        <v>26</v>
+      </c>
+      <c r="E85" t="s">
+        <v>200</v>
+      </c>
+      <c r="F85" s="1">
+        <v>44833.886087962965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to send connection only 500+ connections
</commit_message>
<xml_diff>
--- a/Docs/Prashant Mewada.xlsx
+++ b/Docs/Prashant Mewada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prashant\Documents\UiPath\LinkedInBot\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6567A271-5143-41CF-BC39-196067AEFF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D83BB39-D5F3-468D-9383-DE6FFC5AC57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="355">
   <si>
     <t>Name</t>
   </si>
@@ -960,6 +960,138 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/divya-c-50b448227</t>
+  </si>
+  <si>
+    <t>Priya Darshini</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/priya-darshini-850448232</t>
+  </si>
+  <si>
+    <t>Priyanka Dash</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/priyanka-dash-7340851a0</t>
+  </si>
+  <si>
+    <t>Pavithra Paritala</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/pavithra-paritala-8578ba250</t>
+  </si>
+  <si>
+    <t>IMRAN SHAIK</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/imran-shaik-4414a5138</t>
+  </si>
+  <si>
+    <t>Divya Dwivedi</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/divya-dwivedi-64a2411b9</t>
+  </si>
+  <si>
+    <t>Revathi Conch</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/revathi-conch-0a880323a</t>
+  </si>
+  <si>
+    <t>Naveen Kumar</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/naveen-kumar-234653b</t>
+  </si>
+  <si>
+    <t>chandrahasa nm</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/chandrahasa-nm-3b568696</t>
+  </si>
+  <si>
+    <t>Ramya Yerramilli</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ramya-yerramilli-0b094918</t>
+  </si>
+  <si>
+    <t>UIPath MVP</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Katrina Y.</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/katrina-y-108294b3</t>
+  </si>
+  <si>
+    <t>Swetha K</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/swethahr</t>
+  </si>
+  <si>
+    <t>Julia Tylers</t>
+  </si>
+  <si>
+    <t>Connect - Not Sent - Connections - 13</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/julia-tylers-709a97213</t>
+  </si>
+  <si>
+    <t>Noor Oberoi</t>
+  </si>
+  <si>
+    <t>Connect - Not Sent - Connections - 39</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/noor-oberoi-01307473</t>
+  </si>
+  <si>
+    <t>Radhika Gowda</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/radhika-gowda-8376202b</t>
+  </si>
+  <si>
+    <t>Senthil Sekar</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/senthil-sekar-8547ba84</t>
+  </si>
+  <si>
+    <t>Divya Kumari K</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/divyanayak</t>
+  </si>
+  <si>
+    <t>Suchitra Balakrishna</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/suchitra-balakrishna-b1545426</t>
+  </si>
+  <si>
+    <t>Santhosh Ranganath</t>
+  </si>
+  <si>
+    <t>Connect - Not Sent - Connections - 311</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/santhosh-ranganath-57550151</t>
+  </si>
+  <si>
+    <t>Priyanka Malhotra</t>
+  </si>
+  <si>
+    <t>Connect - Not Sent - Connections - 168</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/priyanka-malhotra-756b8495</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1341,13 +1473,13 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1">
-        <v>44839.886736111112</v>
+        <v>44841.962175925924</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1364,10 +1496,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="1">
-        <v>44839.894606481481</v>
+        <v>44841.921180555553</v>
       </c>
       <c r="F4" t="s">
-        <v>270</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1498,15 +1630,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H139"/>
+  <dimension ref="A1:H158"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="H141" sqref="H141"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
@@ -4081,6 +4215,386 @@
       </c>
       <c r="F139" s="1">
         <v>44839.894293981481</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>311</v>
+      </c>
+      <c r="B140" t="s">
+        <v>15</v>
+      </c>
+      <c r="C140" t="s">
+        <v>12</v>
+      </c>
+      <c r="D140" t="s">
+        <v>25</v>
+      </c>
+      <c r="E140" t="s">
+        <v>312</v>
+      </c>
+      <c r="F140" s="1">
+        <v>44841.917442129627</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>313</v>
+      </c>
+      <c r="B141" t="s">
+        <v>15</v>
+      </c>
+      <c r="C141" t="s">
+        <v>12</v>
+      </c>
+      <c r="D141" t="s">
+        <v>27</v>
+      </c>
+      <c r="E141" t="s">
+        <v>314</v>
+      </c>
+      <c r="F141" s="1">
+        <v>44841.917685185188</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>315</v>
+      </c>
+      <c r="B142" t="s">
+        <v>15</v>
+      </c>
+      <c r="C142" t="s">
+        <v>12</v>
+      </c>
+      <c r="D142" t="s">
+        <v>25</v>
+      </c>
+      <c r="E142" t="s">
+        <v>316</v>
+      </c>
+      <c r="F142" s="1">
+        <v>44841.918078703704</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>317</v>
+      </c>
+      <c r="B143" t="s">
+        <v>15</v>
+      </c>
+      <c r="C143" t="s">
+        <v>12</v>
+      </c>
+      <c r="D143" t="s">
+        <v>27</v>
+      </c>
+      <c r="E143" t="s">
+        <v>318</v>
+      </c>
+      <c r="F143" s="1">
+        <v>44841.918599537035</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>319</v>
+      </c>
+      <c r="B144" t="s">
+        <v>15</v>
+      </c>
+      <c r="C144" t="s">
+        <v>12</v>
+      </c>
+      <c r="D144" t="s">
+        <v>25</v>
+      </c>
+      <c r="E144" t="s">
+        <v>320</v>
+      </c>
+      <c r="F144" s="1">
+        <v>44841.918993055559</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>321</v>
+      </c>
+      <c r="B145" t="s">
+        <v>15</v>
+      </c>
+      <c r="C145" t="s">
+        <v>12</v>
+      </c>
+      <c r="D145" t="s">
+        <v>25</v>
+      </c>
+      <c r="E145" t="s">
+        <v>322</v>
+      </c>
+      <c r="F145" s="1">
+        <v>44841.919421296298</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>323</v>
+      </c>
+      <c r="B146" t="s">
+        <v>15</v>
+      </c>
+      <c r="C146" t="s">
+        <v>12</v>
+      </c>
+      <c r="D146" t="s">
+        <v>30</v>
+      </c>
+      <c r="E146" t="s">
+        <v>324</v>
+      </c>
+      <c r="F146" s="1">
+        <v>44841.919814814813</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>325</v>
+      </c>
+      <c r="B147" t="s">
+        <v>15</v>
+      </c>
+      <c r="C147" t="s">
+        <v>12</v>
+      </c>
+      <c r="D147" t="s">
+        <v>30</v>
+      </c>
+      <c r="E147" t="s">
+        <v>326</v>
+      </c>
+      <c r="F147" s="1">
+        <v>44841.920173611114</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>327</v>
+      </c>
+      <c r="B148" t="s">
+        <v>15</v>
+      </c>
+      <c r="C148" t="s">
+        <v>12</v>
+      </c>
+      <c r="D148" t="s">
+        <v>30</v>
+      </c>
+      <c r="E148" t="s">
+        <v>328</v>
+      </c>
+      <c r="F148" s="1">
+        <v>44841.920914351853</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>331</v>
+      </c>
+      <c r="B149" t="s">
+        <v>329</v>
+      </c>
+      <c r="C149" t="s">
+        <v>330</v>
+      </c>
+      <c r="D149" t="s">
+        <v>44</v>
+      </c>
+      <c r="E149" t="s">
+        <v>332</v>
+      </c>
+      <c r="F149" s="1">
+        <v>44841.955740740741</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>333</v>
+      </c>
+      <c r="B150" t="s">
+        <v>11</v>
+      </c>
+      <c r="C150" t="s">
+        <v>12</v>
+      </c>
+      <c r="D150" t="s">
+        <v>25</v>
+      </c>
+      <c r="E150" t="s">
+        <v>334</v>
+      </c>
+      <c r="F150" s="1">
+        <v>44841.960196759261</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>335</v>
+      </c>
+      <c r="B151" t="s">
+        <v>11</v>
+      </c>
+      <c r="C151" t="s">
+        <v>12</v>
+      </c>
+      <c r="D151" t="s">
+        <v>336</v>
+      </c>
+      <c r="E151" t="s">
+        <v>337</v>
+      </c>
+      <c r="F151" s="1">
+        <v>44841.960312499999</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>338</v>
+      </c>
+      <c r="B152" t="s">
+        <v>11</v>
+      </c>
+      <c r="C152" t="s">
+        <v>12</v>
+      </c>
+      <c r="D152" t="s">
+        <v>339</v>
+      </c>
+      <c r="E152" t="s">
+        <v>340</v>
+      </c>
+      <c r="F152" s="1">
+        <v>44841.960428240738</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>341</v>
+      </c>
+      <c r="B153" t="s">
+        <v>11</v>
+      </c>
+      <c r="C153" t="s">
+        <v>12</v>
+      </c>
+      <c r="D153" t="s">
+        <v>30</v>
+      </c>
+      <c r="E153" t="s">
+        <v>342</v>
+      </c>
+      <c r="F153" s="1">
+        <v>44841.960752314815</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>343</v>
+      </c>
+      <c r="B154" t="s">
+        <v>11</v>
+      </c>
+      <c r="C154" t="s">
+        <v>12</v>
+      </c>
+      <c r="D154" t="s">
+        <v>30</v>
+      </c>
+      <c r="E154" t="s">
+        <v>344</v>
+      </c>
+      <c r="F154" s="1">
+        <v>44841.961087962962</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>345</v>
+      </c>
+      <c r="B155" t="s">
+        <v>11</v>
+      </c>
+      <c r="C155" t="s">
+        <v>12</v>
+      </c>
+      <c r="D155" t="s">
+        <v>30</v>
+      </c>
+      <c r="E155" t="s">
+        <v>346</v>
+      </c>
+      <c r="F155" s="1">
+        <v>44841.961435185185</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>347</v>
+      </c>
+      <c r="B156" t="s">
+        <v>11</v>
+      </c>
+      <c r="C156" t="s">
+        <v>12</v>
+      </c>
+      <c r="D156" t="s">
+        <v>30</v>
+      </c>
+      <c r="E156" t="s">
+        <v>348</v>
+      </c>
+      <c r="F156" s="1">
+        <v>44841.961782407408</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>349</v>
+      </c>
+      <c r="B157" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" t="s">
+        <v>12</v>
+      </c>
+      <c r="D157" t="s">
+        <v>350</v>
+      </c>
+      <c r="E157" t="s">
+        <v>351</v>
+      </c>
+      <c r="F157" s="1">
+        <v>44841.961898148147</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>352</v>
+      </c>
+      <c r="B158" t="s">
+        <v>11</v>
+      </c>
+      <c r="C158" t="s">
+        <v>12</v>
+      </c>
+      <c r="D158" t="s">
+        <v>353</v>
+      </c>
+      <c r="E158" t="s">
+        <v>354</v>
+      </c>
+      <c r="F158" s="1">
+        <v>44841.962013888886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>